<commit_message>
A revisão da Doc, mais a tabela dos Riscos
</commit_message>
<xml_diff>
--- a/Documentação/Riscos do projeto.xlsx
+++ b/Documentação/Riscos do projeto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Desktop\Arquivos temporários\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a54cf72ee4da13f0/Área de Trabalho/Faculdade ADS/arquivos_projeto/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CE75F1-FF38-4A55-A3E4-0ACEF0D5D3DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{03CE75F1-FF38-4A55-A3E4-0ACEF0D5D3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F2AB510-994C-4704-AE01-C84B2E27AA78}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha 1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Risco</t>
   </si>
@@ -85,6 +85,33 @@
   </si>
   <si>
     <t>Ter rotina de backups constantes do repositório no computador de cada um dos membros da equipe.</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Grande</t>
+  </si>
+  <si>
+    <t>Gravíssimo</t>
+  </si>
+  <si>
+    <t>Leve</t>
+  </si>
+  <si>
+    <t>Cada integrante deve se ajudar a cobrir a falta do integrante dividindo a apresentação</t>
+  </si>
+  <si>
+    <t>Avisar sobre as consequencias de seus atos para o próprio tomar uma atitude, caso não resolva, levar o fato para os superiores</t>
+  </si>
+  <si>
+    <t>Comunicar com o grupo sobre tal problema e, caso necessário, afastamento temporario das atividades</t>
   </si>
 </sst>
 </file>
@@ -155,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -235,44 +262,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -590,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:K3"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,36 +666,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="7" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7" t="s">
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="8" t="s">
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="S1" s="9"/>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="U1" s="10"/>
@@ -641,247 +703,302 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
       <c r="Y1" s="9"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="3"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="11" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="3"/>
+      <c r="T2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
     </row>
     <row r="3" spans="1:27" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="11" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="4" t="s">
+      <c r="S3" s="3"/>
+      <c r="T3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
     </row>
-    <row r="4" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:27" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="11" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="14"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="11"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
     </row>
-    <row r="5" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:27" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="11" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="11"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
     </row>
     <row r="6" spans="1:27" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="11" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="14"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="11"/>
-      <c r="T6" s="4" t="s">
+      <c r="S6" s="3"/>
+      <c r="T6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
     </row>
-    <row r="7" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:27" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="11" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="11"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="11" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="11"/>
-      <c r="T8" s="4" t="s">
+      <c r="S8" s="3"/>
+      <c r="T8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:Y7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:Y8"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:Y6"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:Y5"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:Y3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:Y2"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="I1:K1"/>
@@ -896,40 +1013,8 @@
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:Y1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:Y2"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:Y3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:Y4"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:Y6"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:Y5"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:Y8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:Y7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
atualizando chave composta no BD e Riscos do projeto
</commit_message>
<xml_diff>
--- a/Documentação/Riscos do projeto.xlsx
+++ b/Documentação/Riscos do projeto.xlsx
@@ -5,22 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a54cf72ee4da13f0/Área de Trabalho/Faculdade ADS/arquivos_projeto/Documentação/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d4688b2ef84ae56b/Área de Trabalho/PESQUISA E INOVAÇÃO/PROJETO_SPRINT2/arquivos_projeto/Documentação/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{03CE75F1-FF38-4A55-A3E4-0ACEF0D5D3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F2AB510-994C-4704-AE01-C84B2E27AA78}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{03CE75F1-FF38-4A55-A3E4-0ACEF0D5D3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28567EA0-817E-424B-88DF-3723C7DDA257}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Risco</t>
   </si>
@@ -84,27 +89,6 @@
     <t>Comunicação com os demais membros da equipe sobre o problema e se possível ter equipamentos alternativos para seguir com os afazeres do projeto (notebook, tablet etc).</t>
   </si>
   <si>
-    <t>Ter rotina de backups constantes do repositório no computador de cada um dos membros da equipe.</t>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Baixa</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Grande</t>
-  </si>
-  <si>
-    <t>Gravíssimo</t>
-  </si>
-  <si>
-    <t>Leve</t>
-  </si>
-  <si>
     <t>Cada integrante deve se ajudar a cobrir a falta do integrante dividindo a apresentação</t>
   </si>
   <si>
@@ -112,6 +96,9 @@
   </si>
   <si>
     <t>Comunicar com o grupo sobre tal problema e, caso necessário, afastamento temporario das atividades</t>
+  </si>
+  <si>
+    <t>Ter rotina de backups constante do repositório no computador de cada um dos membros da equipe.</t>
   </si>
 </sst>
 </file>
@@ -157,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +168,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -291,50 +290,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -654,55 +659,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:Q2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="32.7109375" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="1" max="25" width="9.28515625" customWidth="1"/>
     <col min="26" max="27" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="4" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4" t="s">
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="5" t="s">
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="5" t="s">
+      <c r="S1" s="10"/>
+      <c r="T1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="9"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="10"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="2"/>
     </row>
@@ -716,32 +720,35 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="3">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="6">
+        <v>3</v>
+      </c>
+      <c r="M2" s="7"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="16">
+        <f>I2*L2</f>
+        <v>6</v>
+      </c>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
       <c r="R2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S2" s="3"/>
-      <c r="T2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
+      <c r="T2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="3" spans="1:27" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -754,31 +761,34 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
+      <c r="I3" s="3">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="3">
+        <v>2</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="17">
+        <f t="shared" ref="O3:O8" si="0">I3*L3</f>
+        <v>4</v>
+      </c>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
       <c r="R3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="S3" s="3"/>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
     </row>
     <row r="4" spans="1:27" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -791,31 +801,34 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
-        <v>20</v>
+      <c r="I4" s="3">
+        <v>1</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
+      <c r="L4" s="6">
+        <v>3</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
       <c r="R4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S4" s="3"/>
-      <c r="T4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
+      <c r="T4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:27" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -828,31 +841,34 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
+      <c r="I5" s="3">
+        <v>1</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
+      <c r="L5" s="6">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
       <c r="R5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S5" s="3"/>
-      <c r="T5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
+      <c r="T5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
     </row>
     <row r="6" spans="1:27" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -865,31 +881,34 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
+      <c r="I6" s="3">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
       <c r="R6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S6" s="3"/>
-      <c r="T6" s="11" t="s">
+      <c r="T6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
     </row>
     <row r="7" spans="1:27" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -902,31 +921,34 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3">
+        <v>2</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
       <c r="R7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S7" s="3"/>
-      <c r="T7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
+      <c r="T7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
     </row>
     <row r="8" spans="1:27" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -939,66 +961,37 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
       <c r="R8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S8" s="3"/>
-      <c r="T8" s="11" t="s">
+      <c r="T8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="T7:Y7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="T8:Y8"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:Y6"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:Y5"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:Y3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:Y4"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:Y1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:Y2"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="I1:K1"/>
@@ -1015,6 +1008,38 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="L6:N6"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:Y2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:Y3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:Y6"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:Y5"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:N8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:Y8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="T7:Y7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>